<commit_message>
update to share with Christopher
</commit_message>
<xml_diff>
--- a/bioprojects/bumblebee_PRJNA533306/SraRunTable.xlsx
+++ b/bioprojects/bumblebee_PRJNA533306/SraRunTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grovesdixon/lab_files/projects/seesaw_test/by_project/bumblebee_PRJNA533306/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grovesdixon/gitreps/invert_meth_and_transcription/bioprojects/bumblebee_PRJNA533306/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39F2418-E124-6247-845A-807EA3BCA532}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE760AC6-DFF9-344D-8847-4D6BA71420DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8260" yWindow="9660" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7680" yWindow="1780" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SraRunTable" sheetId="1" r:id="rId1"/>
@@ -752,7 +752,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -932,6 +932,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1093,10 +1099,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1454,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8:L25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2388,119 +2397,119 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>200</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="3">
         <v>2449</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="3">
         <v>892</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="3">
         <v>24</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="S9" t="s">
+      <c r="S9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="3">
         <v>0</v>
       </c>
-      <c r="V9" t="s">
+      <c r="V9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="W9" t="s">
+      <c r="W9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="X9" t="s">
+      <c r="X9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Y9" s="1">
-        <v>43574</v>
-      </c>
-      <c r="Z9" t="s">
+      <c r="Y9" s="4">
+        <v>43574</v>
+      </c>
+      <c r="Z9" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AA9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AB9" s="1">
-        <v>43574</v>
-      </c>
-      <c r="AC9" t="s">
+      <c r="AB9" s="4">
+        <v>43574</v>
+      </c>
+      <c r="AC9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AD9" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AE9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF9" s="2">
+      <c r="AE9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF9" s="5">
         <v>42370</v>
       </c>
-      <c r="AG9" t="s">
+      <c r="AG9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="AH9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK9" t="s">
+      <c r="AH9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AL9" t="s">
+      <c r="AL9" s="3" t="s">
         <v>63</v>
       </c>
     </row>
@@ -4464,7 +4473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C986102D-E73E-4441-AD8B-93BA6C95933D}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>